<commit_message>
ch-atc version 3.2.0 on 2024-01-31
</commit_message>
<xml_diff>
--- a/ig/ch-atc/ValueSet-DocumentAuditEventType.xlsx
+++ b/ig/ch-atc/ValueSet-DocumentAuditEventType.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.2.0-ballot</t>
+    <t>3.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>ATC_DOC_SEARCH</t>
-  </si>
-  <si>
-    <t>Document search</t>
   </si>
   <si>
     <t/>
@@ -449,24 +446,22 @@
       <c r="A6" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="B6" t="s" s="2">
-        <v>34</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>36</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>